<commit_message>
updated example rules and tests
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/power-grid-example.xlsx
+++ b/cognite/neat/rules/examples/power-grid-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594EE73-B057-2946-8882-C9F604A1EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10ED594D-6C70-2D4C-A640-9255C31D720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45860" yWindow="500" windowWidth="22940" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
-  <si>
-    <t>shortName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t>version</t>
   </si>
   <si>
     <t>0.1.0</t>
-  </si>
-  <si>
-    <t>isCurrentVersion</t>
   </si>
   <si>
     <t>created</t>
@@ -233,9 +227,6 @@
     <t>Dataset Id</t>
   </si>
   <si>
-    <t>dataSetId</t>
-  </si>
-  <si>
     <t>cim:SubGeographicalRegion(cim:IdentifiedObject.name)</t>
   </si>
   <si>
@@ -243,9 +234,6 @@
   </si>
   <si>
     <t>cim:GeographicalRegion(cim:IdentifiedObject.name)</t>
-  </si>
-  <si>
-    <t>2626756768281823</t>
   </si>
   <si>
     <t>Asset, Relationship</t>
@@ -267,9 +255,6 @@
   </si>
   <si>
     <t>http://purl.org/nordic44#</t>
-  </si>
-  <si>
-    <t>externalIdPrefix</t>
   </si>
   <si>
     <t>dct</t>
@@ -663,6 +648,9 @@
   <si>
     <t>The alternative name that identifies Substation</t>
   </si>
+  <si>
+    <t>prefix</t>
+  </si>
 </sst>
 </file>
 
@@ -671,7 +659,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -840,12 +828,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1050,9 +1032,9 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1063,9 +1045,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1089,7 +1068,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1116,7 +1094,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1127,7 +1105,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1137,7 +1115,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,9 +1477,9 @@
     <tabColor rgb="FFFFE699"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W996"/>
+  <dimension ref="A1:W993"/>
   <sheetViews>
-    <sheetView zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1520,10 +1498,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1549,10 +1527,10 @@
     </row>
     <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -1576,26 +1554,26 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="B3" s="8" t="b">
-        <v>1</v>
+      <c r="B3" s="8">
+        <v>44833</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1607,10 +1585,10 @@
     </row>
     <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B4" s="9">
-        <v>44833</v>
+      <c r="B4" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
@@ -1636,10 +1614,10 @@
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1665,10 +1643,10 @@
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1692,18 +1670,18 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1722,25 +1700,21 @@
       <c r="W7" s="4"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1751,12 +1725,8 @@
       <c r="W8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1780,10 +1750,8 @@
       <c r="W9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -26381,81 +26349,6 @@
       <c r="V993" s="4"/>
       <c r="W993" s="4"/>
     </row>
-    <row r="994" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A994" s="4"/>
-      <c r="B994" s="4"/>
-      <c r="C994" s="4"/>
-      <c r="D994" s="4"/>
-      <c r="E994" s="4"/>
-      <c r="F994" s="4"/>
-      <c r="G994" s="4"/>
-      <c r="H994" s="4"/>
-      <c r="I994" s="4"/>
-      <c r="J994" s="4"/>
-      <c r="K994" s="4"/>
-      <c r="L994" s="4"/>
-      <c r="M994" s="4"/>
-      <c r="N994" s="4"/>
-      <c r="O994" s="4"/>
-      <c r="P994" s="4"/>
-      <c r="Q994" s="4"/>
-      <c r="R994" s="4"/>
-      <c r="S994" s="4"/>
-      <c r="T994" s="4"/>
-      <c r="U994" s="4"/>
-      <c r="V994" s="4"/>
-      <c r="W994" s="4"/>
-    </row>
-    <row r="995" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A995" s="4"/>
-      <c r="B995" s="4"/>
-      <c r="C995" s="4"/>
-      <c r="D995" s="4"/>
-      <c r="E995" s="4"/>
-      <c r="F995" s="4"/>
-      <c r="G995" s="4"/>
-      <c r="H995" s="4"/>
-      <c r="I995" s="4"/>
-      <c r="J995" s="4"/>
-      <c r="K995" s="4"/>
-      <c r="L995" s="4"/>
-      <c r="M995" s="4"/>
-      <c r="N995" s="4"/>
-      <c r="O995" s="4"/>
-      <c r="P995" s="4"/>
-      <c r="Q995" s="4"/>
-      <c r="R995" s="4"/>
-      <c r="S995" s="4"/>
-      <c r="T995" s="4"/>
-      <c r="U995" s="4"/>
-      <c r="V995" s="4"/>
-      <c r="W995" s="4"/>
-    </row>
-    <row r="996" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="4"/>
-      <c r="B996" s="4"/>
-      <c r="C996" s="4"/>
-      <c r="D996" s="4"/>
-      <c r="E996" s="4"/>
-      <c r="F996" s="4"/>
-      <c r="G996" s="4"/>
-      <c r="H996" s="4"/>
-      <c r="I996" s="4"/>
-      <c r="J996" s="4"/>
-      <c r="K996" s="4"/>
-      <c r="L996" s="4"/>
-      <c r="M996" s="4"/>
-      <c r="N996" s="4"/>
-      <c r="O996" s="4"/>
-      <c r="P996" s="4"/>
-      <c r="Q996" s="4"/>
-      <c r="R996" s="4"/>
-      <c r="S996" s="4"/>
-      <c r="T996" s="4"/>
-      <c r="U996" s="4"/>
-      <c r="V996" s="4"/>
-      <c r="W996" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -26470,7 +26363,7 @@
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -26491,198 +26384,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>56</v>
+      <c r="A1" s="48" t="s">
+        <v>54</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="50"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="53" t="s">
-        <v>59</v>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-    </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>45</v>
+      <c r="E2" s="14" t="s">
+        <v>52</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>46</v>
+      <c r="F2" s="14" t="s">
+        <v>66</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>54</v>
+      <c r="G2" s="15" t="s">
+        <v>8</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>68</v>
+      <c r="H2" s="15" t="s">
+        <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -26735,443 +26628,443 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="55" t="s">
-        <v>66</v>
+      <c r="N1" s="52"/>
+      <c r="O1" s="51" t="s">
+        <v>57</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+    </row>
+    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="53" t="s">
-        <v>59</v>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>14</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-    </row>
-    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>43</v>
+      <c r="B7" s="17" t="s">
+        <v>98</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>47</v>
+      <c r="C7" s="18" t="s">
+        <v>21</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>48</v>
+      <c r="E7" s="19">
+        <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F7" s="19">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>50</v>
+      <c r="N7" s="31" t="s">
+        <v>39</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>46</v>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>19</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="B8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="29">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="29">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="28">
-        <v>1</v>
+      <c r="L10" s="28"/>
+      <c r="M10" s="46" t="s">
+        <v>49</v>
       </c>
-      <c r="F3" s="28">
-        <v>1</v>
+      <c r="N10" s="45" t="s">
+        <v>101</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="25">
-        <v>1</v>
-      </c>
-      <c r="F4" s="25">
-        <v>1</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="25">
-        <v>1</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-    </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="31">
-        <v>1</v>
-      </c>
-      <c r="F8" s="31">
-        <v>1</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="31">
-        <v>1</v>
-      </c>
-      <c r="F9" s="31">
-        <v>1</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="31">
-        <v>1</v>
-      </c>
-      <c r="F10" s="31">
-        <v>1</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="30"/>
-      <c r="M10" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N12" s="49"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="13"/>
-      <c r="N14" s="49"/>
+      <c r="C14" s="12"/>
+      <c r="N14" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -27204,21 +27097,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>76</v>
+      <c r="A1" s="55" t="s">
+        <v>72</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>77</v>
+      <c r="A2" s="30" t="s">
+        <v>73</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>47</v>
+      <c r="B2" s="30" t="s">
+        <v>45</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>78</v>
+      <c r="C2" s="30" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -27247,129 +27140,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B5" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>87</v>
+      <c r="C5" s="44" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>39</v>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>27</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>40</v>
+      <c r="B6" s="38" t="s">
+        <v>28</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>93</v>
+      <c r="C6" s="44" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="42" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>92</v>
+    </row>
+    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41" t="s">
+        <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>82</v>
+      <c r="B11" s="40" t="s">
+        <v>76</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>83</v>
+      <c r="C11" s="43" t="s">
+        <v>86</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Feature from strings to things part 3 (#218)
## [0.49.0] - 05-12-23

## Deprecated
- `data_set_id`, `cdfSpaceName`, `externalIdPrefix` in `Metadata` sheet has been removed

## Improved
- `Metadata` sheet now contains only two mandatory fields, namely: `prefix` (i.e., `space`), `version`, other fields are optional or generated automatically
- Generation of `Labels`, `Asset` and `Relationship` requires explicit configuration of `data_set_id` and external id prefixes, enabling reuse of same rules for multiple data sets
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/power-grid-example.xlsx
+++ b/cognite/neat/rules/examples/power-grid-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594EE73-B057-2946-8882-C9F604A1EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10ED594D-6C70-2D4C-A640-9255C31D720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45860" yWindow="500" windowWidth="22940" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
-  <si>
-    <t>shortName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t>version</t>
   </si>
   <si>
     <t>0.1.0</t>
-  </si>
-  <si>
-    <t>isCurrentVersion</t>
   </si>
   <si>
     <t>created</t>
@@ -233,9 +227,6 @@
     <t>Dataset Id</t>
   </si>
   <si>
-    <t>dataSetId</t>
-  </si>
-  <si>
     <t>cim:SubGeographicalRegion(cim:IdentifiedObject.name)</t>
   </si>
   <si>
@@ -243,9 +234,6 @@
   </si>
   <si>
     <t>cim:GeographicalRegion(cim:IdentifiedObject.name)</t>
-  </si>
-  <si>
-    <t>2626756768281823</t>
   </si>
   <si>
     <t>Asset, Relationship</t>
@@ -267,9 +255,6 @@
   </si>
   <si>
     <t>http://purl.org/nordic44#</t>
-  </si>
-  <si>
-    <t>externalIdPrefix</t>
   </si>
   <si>
     <t>dct</t>
@@ -663,6 +648,9 @@
   <si>
     <t>The alternative name that identifies Substation</t>
   </si>
+  <si>
+    <t>prefix</t>
+  </si>
 </sst>
 </file>
 
@@ -671,7 +659,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -840,12 +828,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1050,9 +1032,9 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1063,9 +1045,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1089,7 +1068,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1116,7 +1094,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1127,7 +1105,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1137,7 +1115,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,9 +1477,9 @@
     <tabColor rgb="FFFFE699"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W996"/>
+  <dimension ref="A1:W993"/>
   <sheetViews>
-    <sheetView zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1520,10 +1498,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1549,10 +1527,10 @@
     </row>
     <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -1576,26 +1554,26 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="B3" s="8" t="b">
-        <v>1</v>
+      <c r="B3" s="8">
+        <v>44833</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1607,10 +1585,10 @@
     </row>
     <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B4" s="9">
-        <v>44833</v>
+      <c r="B4" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
@@ -1636,10 +1614,10 @@
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1665,10 +1643,10 @@
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1692,18 +1670,18 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1722,25 +1700,21 @@
       <c r="W7" s="4"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1751,12 +1725,8 @@
       <c r="W8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1780,10 +1750,8 @@
       <c r="W9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -26381,81 +26349,6 @@
       <c r="V993" s="4"/>
       <c r="W993" s="4"/>
     </row>
-    <row r="994" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A994" s="4"/>
-      <c r="B994" s="4"/>
-      <c r="C994" s="4"/>
-      <c r="D994" s="4"/>
-      <c r="E994" s="4"/>
-      <c r="F994" s="4"/>
-      <c r="G994" s="4"/>
-      <c r="H994" s="4"/>
-      <c r="I994" s="4"/>
-      <c r="J994" s="4"/>
-      <c r="K994" s="4"/>
-      <c r="L994" s="4"/>
-      <c r="M994" s="4"/>
-      <c r="N994" s="4"/>
-      <c r="O994" s="4"/>
-      <c r="P994" s="4"/>
-      <c r="Q994" s="4"/>
-      <c r="R994" s="4"/>
-      <c r="S994" s="4"/>
-      <c r="T994" s="4"/>
-      <c r="U994" s="4"/>
-      <c r="V994" s="4"/>
-      <c r="W994" s="4"/>
-    </row>
-    <row r="995" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A995" s="4"/>
-      <c r="B995" s="4"/>
-      <c r="C995" s="4"/>
-      <c r="D995" s="4"/>
-      <c r="E995" s="4"/>
-      <c r="F995" s="4"/>
-      <c r="G995" s="4"/>
-      <c r="H995" s="4"/>
-      <c r="I995" s="4"/>
-      <c r="J995" s="4"/>
-      <c r="K995" s="4"/>
-      <c r="L995" s="4"/>
-      <c r="M995" s="4"/>
-      <c r="N995" s="4"/>
-      <c r="O995" s="4"/>
-      <c r="P995" s="4"/>
-      <c r="Q995" s="4"/>
-      <c r="R995" s="4"/>
-      <c r="S995" s="4"/>
-      <c r="T995" s="4"/>
-      <c r="U995" s="4"/>
-      <c r="V995" s="4"/>
-      <c r="W995" s="4"/>
-    </row>
-    <row r="996" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="4"/>
-      <c r="B996" s="4"/>
-      <c r="C996" s="4"/>
-      <c r="D996" s="4"/>
-      <c r="E996" s="4"/>
-      <c r="F996" s="4"/>
-      <c r="G996" s="4"/>
-      <c r="H996" s="4"/>
-      <c r="I996" s="4"/>
-      <c r="J996" s="4"/>
-      <c r="K996" s="4"/>
-      <c r="L996" s="4"/>
-      <c r="M996" s="4"/>
-      <c r="N996" s="4"/>
-      <c r="O996" s="4"/>
-      <c r="P996" s="4"/>
-      <c r="Q996" s="4"/>
-      <c r="R996" s="4"/>
-      <c r="S996" s="4"/>
-      <c r="T996" s="4"/>
-      <c r="U996" s="4"/>
-      <c r="V996" s="4"/>
-      <c r="W996" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -26470,7 +26363,7 @@
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -26491,198 +26384,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>56</v>
+      <c r="A1" s="48" t="s">
+        <v>54</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="50"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="53" t="s">
-        <v>59</v>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-    </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>45</v>
+      <c r="E2" s="14" t="s">
+        <v>52</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>46</v>
+      <c r="F2" s="14" t="s">
+        <v>66</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>54</v>
+      <c r="G2" s="15" t="s">
+        <v>8</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>68</v>
+      <c r="H2" s="15" t="s">
+        <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -26735,443 +26628,443 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="55" t="s">
-        <v>66</v>
+      <c r="N1" s="52"/>
+      <c r="O1" s="51" t="s">
+        <v>57</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+    </row>
+    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="53" t="s">
-        <v>59</v>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>14</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-    </row>
-    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>43</v>
+      <c r="B7" s="17" t="s">
+        <v>98</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>47</v>
+      <c r="C7" s="18" t="s">
+        <v>21</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>48</v>
+      <c r="E7" s="19">
+        <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F7" s="19">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>50</v>
+      <c r="N7" s="31" t="s">
+        <v>39</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>46</v>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>19</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="B8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="29">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="29">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="28">
-        <v>1</v>
+      <c r="L10" s="28"/>
+      <c r="M10" s="46" t="s">
+        <v>49</v>
       </c>
-      <c r="F3" s="28">
-        <v>1</v>
+      <c r="N10" s="45" t="s">
+        <v>101</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="25">
-        <v>1</v>
-      </c>
-      <c r="F4" s="25">
-        <v>1</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="25">
-        <v>1</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-    </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="31">
-        <v>1</v>
-      </c>
-      <c r="F8" s="31">
-        <v>1</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="31">
-        <v>1</v>
-      </c>
-      <c r="F9" s="31">
-        <v>1</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="31">
-        <v>1</v>
-      </c>
-      <c r="F10" s="31">
-        <v>1</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="30"/>
-      <c r="M10" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N12" s="49"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="13"/>
-      <c r="N14" s="49"/>
+      <c r="C14" s="12"/>
+      <c r="N14" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -27204,21 +27097,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>76</v>
+      <c r="A1" s="55" t="s">
+        <v>72</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>77</v>
+      <c r="A2" s="30" t="s">
+        <v>73</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>47</v>
+      <c r="B2" s="30" t="s">
+        <v>45</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>78</v>
+      <c r="C2" s="30" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -27247,129 +27140,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B5" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>87</v>
+      <c r="C5" s="44" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>39</v>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>27</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>40</v>
+      <c r="B6" s="38" t="s">
+        <v>28</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>93</v>
+      <c r="C6" s="44" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="42" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>92</v>
+    </row>
+    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41" t="s">
+        <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>82</v>
+      <c r="B11" s="40" t="s">
+        <v>76</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>83</v>
+      <c r="C11" s="43" t="s">
+        <v>86</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>